<commit_message>
Fixed few bugs and add 'Unique Institutions' to calculate
</commit_message>
<xml_diff>
--- a/Data/institution_data.xlsx
+++ b/Data/institution_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="330">
   <si>
     <t>Institution</t>
   </si>
@@ -779,6 +779,12 @@
   </si>
   <si>
     <t>McMaster University</t>
+  </si>
+  <si>
+    <t>Australian Synchrotron Project</t>
+  </si>
+  <si>
+    <t>University of California, Davis</t>
   </si>
   <si>
     <t>Australia</t>
@@ -1355,7 +1361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C253"/>
+  <dimension ref="A1:C255"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1377,7 +1383,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1385,7 +1391,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1393,7 +1399,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1401,7 +1407,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1409,7 +1415,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1417,7 +1423,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1425,7 +1431,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1433,7 +1439,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1441,7 +1447,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1449,7 +1455,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1457,7 +1463,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1465,7 +1471,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1473,7 +1479,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1481,7 +1487,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1489,7 +1495,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1497,7 +1503,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1505,7 +1511,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1513,7 +1519,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1521,7 +1527,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1529,7 +1535,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1537,7 +1543,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1545,7 +1551,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1553,7 +1559,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1561,7 +1567,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1569,7 +1575,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1577,7 +1583,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1585,7 +1591,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1593,7 +1599,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1601,7 +1607,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1609,7 +1615,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1617,7 +1623,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1625,7 +1631,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1633,7 +1639,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1641,7 +1647,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1649,7 +1655,7 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1657,7 +1663,7 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1665,7 +1671,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1673,7 +1679,7 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1681,7 +1687,7 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1689,7 +1695,7 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1697,7 +1703,7 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1705,7 +1711,7 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1713,7 +1719,7 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1721,7 +1727,7 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1729,7 +1735,7 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1737,7 +1743,7 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1745,10 +1751,10 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C48" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1756,10 +1762,10 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C49" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1767,10 +1773,10 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C50" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1778,10 +1784,10 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C51" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1789,10 +1795,10 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C52" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1800,10 +1806,10 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C53" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1811,10 +1817,10 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C54" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1822,10 +1828,10 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C55" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1833,10 +1839,10 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C56" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1844,10 +1850,10 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C57" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1855,10 +1861,10 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C58" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1866,10 +1872,10 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C59" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1877,10 +1883,10 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C60" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1888,10 +1894,10 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C61" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1899,10 +1905,10 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C62" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1910,10 +1916,10 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C63" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1921,10 +1927,10 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C64" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1932,10 +1938,10 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C65" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1943,10 +1949,10 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C66" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1954,10 +1960,10 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C67" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1965,10 +1971,10 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C68" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1976,10 +1982,10 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C69" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1987,10 +1993,10 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C70" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1998,10 +2004,10 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C71" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2009,10 +2015,10 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C72" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2020,10 +2026,10 @@
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C73" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2031,10 +2037,10 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C74" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2042,10 +2048,10 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C75" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2053,10 +2059,10 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C76" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2064,10 +2070,10 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C77" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2075,10 +2081,10 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C78" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2086,10 +2092,10 @@
         <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C79" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2097,10 +2103,10 @@
         <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C80" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2108,10 +2114,10 @@
         <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C81" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2119,10 +2125,10 @@
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C82" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2130,10 +2136,10 @@
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C83" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2141,10 +2147,10 @@
         <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C84" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2152,10 +2158,10 @@
         <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C85" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2163,10 +2169,10 @@
         <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C86" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2174,10 +2180,10 @@
         <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C87" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2185,10 +2191,10 @@
         <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C88" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2196,10 +2202,10 @@
         <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C89" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2207,10 +2213,10 @@
         <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C90" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2218,10 +2224,10 @@
         <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C91" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2229,10 +2235,10 @@
         <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C92" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2240,10 +2246,10 @@
         <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C93" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2251,10 +2257,10 @@
         <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C94" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2262,10 +2268,10 @@
         <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C95" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2273,10 +2279,10 @@
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C96" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2284,10 +2290,10 @@
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C97" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2295,10 +2301,10 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C98" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2306,10 +2312,10 @@
         <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C99" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2317,10 +2323,10 @@
         <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C100" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2328,10 +2334,10 @@
         <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C101" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2339,10 +2345,10 @@
         <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C102" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2350,10 +2356,10 @@
         <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C103" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2361,10 +2367,10 @@
         <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C104" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2372,10 +2378,10 @@
         <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C105" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2383,10 +2389,10 @@
         <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C106" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2394,10 +2400,10 @@
         <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C107" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2405,10 +2411,10 @@
         <v>109</v>
       </c>
       <c r="B108" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C108" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2416,10 +2422,10 @@
         <v>110</v>
       </c>
       <c r="B109" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C109" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2427,10 +2433,10 @@
         <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C110" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2438,10 +2444,10 @@
         <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C111" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2449,10 +2455,10 @@
         <v>113</v>
       </c>
       <c r="B112" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C112" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2460,10 +2466,10 @@
         <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C113" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2471,10 +2477,10 @@
         <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C114" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2482,10 +2488,10 @@
         <v>116</v>
       </c>
       <c r="B115" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C115" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2493,10 +2499,10 @@
         <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C116" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2504,10 +2510,10 @@
         <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C117" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2515,10 +2521,10 @@
         <v>119</v>
       </c>
       <c r="B118" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C118" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2526,10 +2532,10 @@
         <v>120</v>
       </c>
       <c r="B119" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C119" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2537,10 +2543,10 @@
         <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C120" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2548,10 +2554,10 @@
         <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C121" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2559,10 +2565,10 @@
         <v>123</v>
       </c>
       <c r="B122" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C122" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2570,10 +2576,10 @@
         <v>124</v>
       </c>
       <c r="B123" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C123" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2581,10 +2587,10 @@
         <v>125</v>
       </c>
       <c r="B124" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C124" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2592,10 +2598,10 @@
         <v>126</v>
       </c>
       <c r="B125" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C125" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2603,10 +2609,10 @@
         <v>127</v>
       </c>
       <c r="B126" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C126" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2614,10 +2620,10 @@
         <v>128</v>
       </c>
       <c r="B127" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C127" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2625,10 +2631,10 @@
         <v>129</v>
       </c>
       <c r="B128" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C128" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2636,10 +2642,10 @@
         <v>130</v>
       </c>
       <c r="B129" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C129" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2647,10 +2653,10 @@
         <v>131</v>
       </c>
       <c r="B130" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C130" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2658,10 +2664,10 @@
         <v>132</v>
       </c>
       <c r="B131" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C131" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2669,10 +2675,10 @@
         <v>133</v>
       </c>
       <c r="B132" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C132" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2680,10 +2686,10 @@
         <v>134</v>
       </c>
       <c r="B133" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C133" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2691,10 +2697,10 @@
         <v>135</v>
       </c>
       <c r="B134" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C134" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2702,10 +2708,10 @@
         <v>136</v>
       </c>
       <c r="B135" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C135" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2713,10 +2719,10 @@
         <v>137</v>
       </c>
       <c r="B136" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C136" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2724,10 +2730,10 @@
         <v>138</v>
       </c>
       <c r="B137" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C137" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2735,10 +2741,10 @@
         <v>139</v>
       </c>
       <c r="B138" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C138" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2746,10 +2752,10 @@
         <v>140</v>
       </c>
       <c r="B139" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C139" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2757,10 +2763,10 @@
         <v>141</v>
       </c>
       <c r="B140" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C140" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2768,10 +2774,10 @@
         <v>142</v>
       </c>
       <c r="B141" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C141" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2779,10 +2785,10 @@
         <v>143</v>
       </c>
       <c r="B142" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C142" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2790,10 +2796,10 @@
         <v>144</v>
       </c>
       <c r="B143" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C143" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2801,10 +2807,10 @@
         <v>145</v>
       </c>
       <c r="B144" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C144" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2812,10 +2818,10 @@
         <v>146</v>
       </c>
       <c r="B145" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C145" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2823,10 +2829,10 @@
         <v>147</v>
       </c>
       <c r="B146" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C146" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2834,10 +2840,10 @@
         <v>148</v>
       </c>
       <c r="B147" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C147" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2845,10 +2851,10 @@
         <v>149</v>
       </c>
       <c r="B148" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C148" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2856,10 +2862,10 @@
         <v>150</v>
       </c>
       <c r="B149" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C149" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2867,10 +2873,10 @@
         <v>151</v>
       </c>
       <c r="B150" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C150" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2878,10 +2884,10 @@
         <v>152</v>
       </c>
       <c r="B151" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C151" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2889,10 +2895,10 @@
         <v>153</v>
       </c>
       <c r="B152" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C152" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2900,10 +2906,10 @@
         <v>154</v>
       </c>
       <c r="B153" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C153" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2911,10 +2917,10 @@
         <v>155</v>
       </c>
       <c r="B154" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C154" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2922,10 +2928,10 @@
         <v>156</v>
       </c>
       <c r="B155" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C155" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2933,10 +2939,10 @@
         <v>157</v>
       </c>
       <c r="B156" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C156" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2944,10 +2950,10 @@
         <v>158</v>
       </c>
       <c r="B157" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C157" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2955,10 +2961,10 @@
         <v>159</v>
       </c>
       <c r="B158" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C158" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2966,10 +2972,10 @@
         <v>160</v>
       </c>
       <c r="B159" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C159" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2977,10 +2983,10 @@
         <v>161</v>
       </c>
       <c r="B160" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C160" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2988,10 +2994,10 @@
         <v>162</v>
       </c>
       <c r="B161" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C161" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2999,10 +3005,10 @@
         <v>163</v>
       </c>
       <c r="B162" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C162" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -3010,10 +3016,10 @@
         <v>164</v>
       </c>
       <c r="B163" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C163" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -3021,10 +3027,10 @@
         <v>165</v>
       </c>
       <c r="B164" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C164" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3032,10 +3038,10 @@
         <v>166</v>
       </c>
       <c r="B165" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C165" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3043,10 +3049,10 @@
         <v>167</v>
       </c>
       <c r="B166" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C166" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3054,10 +3060,10 @@
         <v>168</v>
       </c>
       <c r="B167" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C167" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3065,10 +3071,10 @@
         <v>169</v>
       </c>
       <c r="B168" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C168" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3076,10 +3082,10 @@
         <v>170</v>
       </c>
       <c r="B169" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C169" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3087,10 +3093,10 @@
         <v>171</v>
       </c>
       <c r="B170" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C170" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3098,7 +3104,7 @@
         <v>172</v>
       </c>
       <c r="B171" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3106,10 +3112,10 @@
         <v>173</v>
       </c>
       <c r="B172" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C172" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3117,10 +3123,10 @@
         <v>174</v>
       </c>
       <c r="B173" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C173" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -3128,10 +3134,10 @@
         <v>175</v>
       </c>
       <c r="B174" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C174" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3139,7 +3145,7 @@
         <v>176</v>
       </c>
       <c r="B175" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -3147,10 +3153,10 @@
         <v>177</v>
       </c>
       <c r="B176" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C176" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3158,7 +3164,7 @@
         <v>178</v>
       </c>
       <c r="B177" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3166,10 +3172,10 @@
         <v>179</v>
       </c>
       <c r="B178" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C178" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -3177,10 +3183,10 @@
         <v>180</v>
       </c>
       <c r="B179" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C179" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3188,7 +3194,7 @@
         <v>181</v>
       </c>
       <c r="B180" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3196,7 +3202,7 @@
         <v>182</v>
       </c>
       <c r="B181" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3204,7 +3210,7 @@
         <v>183</v>
       </c>
       <c r="B182" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -3212,10 +3218,10 @@
         <v>184</v>
       </c>
       <c r="B183" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C183" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3223,7 +3229,7 @@
         <v>185</v>
       </c>
       <c r="B184" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3231,7 +3237,7 @@
         <v>186</v>
       </c>
       <c r="B185" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3239,7 +3245,7 @@
         <v>187</v>
       </c>
       <c r="B186" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3247,7 +3253,7 @@
         <v>188</v>
       </c>
       <c r="B187" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3255,10 +3261,10 @@
         <v>189</v>
       </c>
       <c r="B188" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C188" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3266,7 +3272,7 @@
         <v>190</v>
       </c>
       <c r="B189" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3274,7 +3280,7 @@
         <v>191</v>
       </c>
       <c r="B190" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3282,7 +3288,7 @@
         <v>192</v>
       </c>
       <c r="B191" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3290,10 +3296,10 @@
         <v>193</v>
       </c>
       <c r="B192" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C192" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3301,10 +3307,10 @@
         <v>194</v>
       </c>
       <c r="B193" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C193" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3312,10 +3318,10 @@
         <v>195</v>
       </c>
       <c r="B194" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C194" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3323,7 +3329,7 @@
         <v>196</v>
       </c>
       <c r="B195" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3331,10 +3337,10 @@
         <v>197</v>
       </c>
       <c r="B196" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C196" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3342,10 +3348,10 @@
         <v>198</v>
       </c>
       <c r="B197" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C197" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3353,7 +3359,7 @@
         <v>199</v>
       </c>
       <c r="B198" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3361,7 +3367,7 @@
         <v>200</v>
       </c>
       <c r="B199" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -3369,10 +3375,10 @@
         <v>201</v>
       </c>
       <c r="B200" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C200" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3380,10 +3386,10 @@
         <v>202</v>
       </c>
       <c r="B201" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C201" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3391,10 +3397,10 @@
         <v>203</v>
       </c>
       <c r="B202" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C202" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -3402,10 +3408,10 @@
         <v>204</v>
       </c>
       <c r="B203" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C203" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3413,10 +3419,10 @@
         <v>205</v>
       </c>
       <c r="B204" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C204" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -3424,7 +3430,7 @@
         <v>206</v>
       </c>
       <c r="B205" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -3432,10 +3438,10 @@
         <v>207</v>
       </c>
       <c r="B206" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C206" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3443,10 +3449,10 @@
         <v>208</v>
       </c>
       <c r="B207" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C207" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3454,7 +3460,7 @@
         <v>209</v>
       </c>
       <c r="B208" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -3462,10 +3468,10 @@
         <v>210</v>
       </c>
       <c r="B209" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C209" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -3473,7 +3479,7 @@
         <v>211</v>
       </c>
       <c r="B210" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -3481,10 +3487,10 @@
         <v>212</v>
       </c>
       <c r="B211" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C211" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -3492,7 +3498,7 @@
         <v>213</v>
       </c>
       <c r="B212" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -3500,10 +3506,10 @@
         <v>214</v>
       </c>
       <c r="B213" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C213" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -3511,7 +3517,7 @@
         <v>215</v>
       </c>
       <c r="B214" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -3519,10 +3525,10 @@
         <v>216</v>
       </c>
       <c r="B215" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C215" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -3530,10 +3536,10 @@
         <v>217</v>
       </c>
       <c r="B216" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C216" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -3541,7 +3547,7 @@
         <v>218</v>
       </c>
       <c r="B217" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -3549,7 +3555,7 @@
         <v>219</v>
       </c>
       <c r="B218" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -3557,10 +3563,10 @@
         <v>220</v>
       </c>
       <c r="B219" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C219" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -3568,10 +3574,10 @@
         <v>221</v>
       </c>
       <c r="B220" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C220" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -3579,10 +3585,10 @@
         <v>222</v>
       </c>
       <c r="B221" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C221" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -3590,7 +3596,7 @@
         <v>223</v>
       </c>
       <c r="B222" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -3598,7 +3604,7 @@
         <v>224</v>
       </c>
       <c r="B223" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -3606,7 +3612,7 @@
         <v>225</v>
       </c>
       <c r="B224" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -3614,7 +3620,7 @@
         <v>226</v>
       </c>
       <c r="B225" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -3622,10 +3628,10 @@
         <v>227</v>
       </c>
       <c r="B226" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C226" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -3633,7 +3639,7 @@
         <v>228</v>
       </c>
       <c r="B227" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3641,7 +3647,7 @@
         <v>229</v>
       </c>
       <c r="B228" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3649,7 +3655,7 @@
         <v>230</v>
       </c>
       <c r="B229" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3657,7 +3663,7 @@
         <v>231</v>
       </c>
       <c r="B230" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3665,7 +3671,7 @@
         <v>232</v>
       </c>
       <c r="B231" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3673,10 +3679,10 @@
         <v>233</v>
       </c>
       <c r="B232" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C232" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3684,10 +3690,10 @@
         <v>234</v>
       </c>
       <c r="B233" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C233" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3695,7 +3701,7 @@
         <v>235</v>
       </c>
       <c r="B234" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3703,7 +3709,7 @@
         <v>236</v>
       </c>
       <c r="B235" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3711,10 +3717,10 @@
         <v>237</v>
       </c>
       <c r="B236" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C236" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3722,10 +3728,10 @@
         <v>238</v>
       </c>
       <c r="B237" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C237" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3733,7 +3739,7 @@
         <v>239</v>
       </c>
       <c r="B238" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3741,7 +3747,7 @@
         <v>240</v>
       </c>
       <c r="B239" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3749,10 +3755,10 @@
         <v>241</v>
       </c>
       <c r="B240" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C240" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3760,7 +3766,7 @@
         <v>242</v>
       </c>
       <c r="B241" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3768,10 +3774,10 @@
         <v>243</v>
       </c>
       <c r="B242" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C242" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3779,7 +3785,7 @@
         <v>244</v>
       </c>
       <c r="B243" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3787,7 +3793,7 @@
         <v>245</v>
       </c>
       <c r="B244" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3795,10 +3801,10 @@
         <v>246</v>
       </c>
       <c r="B245" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C245" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3806,7 +3812,7 @@
         <v>247</v>
       </c>
       <c r="B246" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3814,10 +3820,10 @@
         <v>248</v>
       </c>
       <c r="B247" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C247" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3825,7 +3831,7 @@
         <v>249</v>
       </c>
       <c r="B248" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3833,7 +3839,7 @@
         <v>250</v>
       </c>
       <c r="B249" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3841,7 +3847,7 @@
         <v>251</v>
       </c>
       <c r="B250" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3849,10 +3855,10 @@
         <v>252</v>
       </c>
       <c r="B251" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C251" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3860,10 +3866,10 @@
         <v>253</v>
       </c>
       <c r="B252" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C252" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3871,7 +3877,26 @@
         <v>254</v>
       </c>
       <c r="B253" t="s">
-        <v>258</v>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" t="s">
+        <v>255</v>
+      </c>
+      <c r="B254" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255" t="s">
+        <v>256</v>
+      </c>
+      <c r="B255" t="s">
+        <v>275</v>
+      </c>
+      <c r="C255" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>